<commit_message>
REFACTOR removed some magic colors from BoardCell
</commit_message>
<xml_diff>
--- a/clueFiles/clueLayout.xlsx
+++ b/clueFiles/clueLayout.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hayden/Documents/Java/ClueGame/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="19480" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14205" windowHeight="7725" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
     <sheet name="PlayerStart" sheetId="5" r:id="rId2"/>
     <sheet name="Plain" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1:AA17"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -654,13 +650,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="R1" zoomScale="140" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="Y1" sqref="Y1:AG9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="24" width="3.1640625" customWidth="1"/>
+    <col min="1" max="24" width="3.140625" customWidth="1"/>
     <col min="26" max="29" width="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2402,12 +2398,12 @@
   <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="24" width="3.1640625" customWidth="1"/>
+    <col min="1" max="24" width="3.140625" customWidth="1"/>
     <col min="26" max="29" width="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4135,13 +4131,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="140" workbookViewId="0">
       <selection activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="24" width="3.1640625" customWidth="1"/>
+    <col min="1" max="24" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">

</xml_diff>